<commit_message>
Testplan um Verbindungen+Attributnamenaenderung erweitert
</commit_message>
<xml_diff>
--- a/Testplan.xlsx
+++ b/Testplan.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\Client\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="243">
   <si>
     <t>Testplan</t>
   </si>
@@ -633,9 +628,6 @@
     <t>Ansicht wird nicht gelöscht und das Popup schließt. Man kehrt zur vorherigen Übersicht zurück.</t>
   </si>
   <si>
-    <t>Verbindungen filtern</t>
-  </si>
-  <si>
     <t>"Auf Änderungen speichern" klicken, "Stadt anzeigen" klicken</t>
   </si>
   <si>
@@ -654,18 +646,9 @@
     <t>"Verbindungen nutzen" klicken</t>
   </si>
   <si>
-    <t>Verbindungen werden aktiviert und können weiter gefiltert werden</t>
-  </si>
-  <si>
     <t>"Verbindungen nutzen" aktiviert</t>
   </si>
   <si>
-    <t>"Eingehende Verbindungen", "Ausgehende Verbindungen" filtern,  "Änderungen speichern" klicken</t>
-  </si>
-  <si>
-    <t>Verbindungen wurden gefiltert und gespeichert. Die aktualiserte Stadt hat nun gefilterte Verbindungen.</t>
-  </si>
-  <si>
     <t>Daten aggregieren</t>
   </si>
   <si>
@@ -730,12 +713,6 @@
   </si>
   <si>
     <t>Alle Ausblendungsvorgänge werden rückgängig gemacht.</t>
-  </si>
-  <si>
-    <t>Es entstehen Straßen zwischen dem ausgewählten Gebäude und allen anderen Gebäude, zu denen eine Verbindung besteht.</t>
-  </si>
-  <si>
-    <t>Noch nicht komplett implementiert. Erfordert noch weitere Anpassung.</t>
   </si>
   <si>
     <t>mehrere Gebäude oder Distrikte wurden geausgeblendet</t>
@@ -765,12 +742,39 @@
   <si>
     <t>Mit der Maus auf einen Vorgarten eines Gebäudes klicken</t>
   </si>
+  <si>
+    <t>Je nach Auswahl von Straßen oder Regenbögen entstehen zwischen dem ausgewählten Gebäude und allen anderen Gebäude Straßen/Regenbögen</t>
+  </si>
+  <si>
+    <t>Verbindungen werden aktiviert und es kann die Darstellungsweise entschieden werden</t>
+  </si>
+  <si>
+    <t>Verbindungsart wählen</t>
+  </si>
+  <si>
+    <t>Entweder die Checkbox "Regenbögen" oder "Straßen" anklicken, "Änderungen speichern" klicken</t>
+  </si>
+  <si>
+    <t>Je nach Wahl, werden in der Stadtansicht die Verbindungen als Straßen oder als Regenbögen dargestellt</t>
+  </si>
+  <si>
+    <t>Attributnamenänderung</t>
+  </si>
+  <si>
+    <t>Die "Legende" ist aufgeklappt</t>
+  </si>
+  <si>
+    <t>Attributnamen ändern in der Legende durch Tastatur Eingabe</t>
+  </si>
+  <si>
+    <t>Der Attributname kann beliebig angepasst werden, speichern ist nicht möglich, nur mit der aktuellen Ansicht URL exportiertbar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,20 +885,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1036,9 +1027,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1057,15 +1045,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1074,6 +1059,12 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1376,7 +1367,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1384,27 +1375,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V91"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F92" sqref="F92"/>
+      <selection pane="bottomRight" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="80.28515625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="6.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="20.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="80.33203125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="33.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="6.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -1425,7 +1416,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1435,44 +1426,44 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="28" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>133</v>
       </c>
@@ -1483,8 +1474,8 @@
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:22" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -1496,26 +1487,26 @@
       <c r="F5" s="32"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="37" t="s">
         <v>189</v>
       </c>
       <c r="F6" s="38"/>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1527,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
@@ -1546,7 +1537,7 @@
       <c r="C8" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="15" t="s">
         <v>91</v>
       </c>
@@ -1557,17 +1548,17 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="15" t="s">
         <v>91</v>
       </c>
@@ -1578,18 +1569,18 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="25" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="24" t="s">
         <v>108</v>
       </c>
       <c r="F10" s="17" t="s">
@@ -1599,18 +1590,18 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="24" t="s">
         <v>108</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -1620,7 +1611,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="11" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
@@ -1633,157 +1624,157 @@
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
     </row>
-    <row r="13" spans="1:22" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="26"/>
+      <c r="E13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="25" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="G13" s="24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="25" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:22" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+    <row r="16" spans="1:22" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="26"/>
+      <c r="E16" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="25" t="s">
+      <c r="D17" s="26"/>
+      <c r="E17" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="24" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="16"/>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="25" t="s">
+      <c r="D18" s="26"/>
+      <c r="E18" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="25" t="s">
+      <c r="D19" s="26"/>
+      <c r="E19" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="24" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="11" customFormat="1" ht="14.4" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>5</v>
+      <c r="B20" s="31" t="s">
+        <v>156</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -1791,405 +1782,405 @@
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
     </row>
-    <row r="21" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+    <row r="21" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="11" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="26"/>
       <c r="E22" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="26"/>
       <c r="E23" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="G23" s="25" t="s">
+    </row>
+    <row r="24" spans="1:7" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="26"/>
+      <c r="E24" s="17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="11" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="F24" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="17" t="s">
+      <c r="B25" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="D25" s="26"/>
+      <c r="E25" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="11" customFormat="1" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="F25" s="25" t="s">
+      <c r="B26" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="F26" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="11" customFormat="1" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="D28" s="26"/>
+      <c r="E28" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="B29" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="B30" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30" s="26"/>
+      <c r="E30" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="F30" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>113</v>
-      </c>
       <c r="B31" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="24"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="24" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+    <row r="32" spans="1:7" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="D32" s="24"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="24" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+    <row r="33" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="24"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="F33" s="25" t="s">
+      <c r="F33" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="G33" s="25" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="G33" s="24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="24"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="F34" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G34" s="24" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="24"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="25" t="s">
+      <c r="F35" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="G35" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+    <row r="36" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="24"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="11" customFormat="1" ht="27" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+    <row r="37" spans="1:7" s="11" customFormat="1" ht="27" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D37" s="20"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="35" t="s">
         <v>149</v>
       </c>
       <c r="F37" s="36"/>
-      <c r="G37" s="25" t="s">
+      <c r="G37" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+    <row r="38" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="24"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="25" t="s">
+      <c r="F38" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="25" t="s">
+      <c r="G38" s="24" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
+    <row r="39" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22" t="s">
         <v>113</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="24"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F39" s="25" t="s">
+      <c r="F39" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+    <row r="40" spans="1:7" s="11" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="14" t="s">
@@ -2201,49 +2192,49 @@
       <c r="F40" s="32"/>
       <c r="G40" s="32"/>
     </row>
-    <row r="41" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+    <row r="41" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25" t="s">
+      <c r="D41" s="23"/>
+      <c r="E41" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="25" t="s">
+      <c r="F41" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="25" t="s">
+      <c r="G41" s="24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+    <row r="42" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="25" t="s">
+      <c r="D42" s="23"/>
+      <c r="E42" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="F42" s="25" t="s">
+      <c r="F42" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="25" t="s">
+      <c r="G42" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A43" s="39"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -2252,7 +2243,7 @@
       <c r="F43" s="39"/>
       <c r="G43" s="39"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
         <v>112</v>
       </c>
@@ -2264,7 +2255,7 @@
       <c r="G44" s="34"/>
     </row>
     <row r="45" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="14" t="s">
@@ -2276,107 +2267,107 @@
       <c r="F45" s="32"/>
       <c r="G45" s="32"/>
     </row>
-    <row r="46" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+    <row r="46" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="25" t="s">
+      <c r="D46" s="23"/>
+      <c r="E46" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="25" t="s">
+      <c r="F46" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G46" s="25" t="s">
+      <c r="G46" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+    <row r="47" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="24"/>
-      <c r="E47" s="25"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="24"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
+    <row r="48" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+    <row r="49" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="25"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
       <c r="F49" s="15"/>
       <c r="G49" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="24" t="s">
+    <row r="50" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="24"/>
-      <c r="E50" s="25"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
       <c r="F50" s="15"/>
       <c r="G50" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+    <row r="51" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="25" t="s">
+      <c r="D51" s="23"/>
+      <c r="E51" s="24" t="s">
         <v>164</v>
       </c>
       <c r="F51" s="15"/>
@@ -2384,25 +2375,25 @@
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
+    <row r="52" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="25"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="24"/>
       <c r="F52" s="15"/>
       <c r="G52" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
+    <row r="53" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B53" s="16" t="s">
@@ -2412,16 +2403,16 @@
         <v>44</v>
       </c>
       <c r="D53" s="17"/>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25" t="s">
+      <c r="F53" s="24"/>
+      <c r="G53" s="24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+    <row r="54" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B54" s="16" t="s">
@@ -2431,41 +2422,41 @@
         <v>100</v>
       </c>
       <c r="D54" s="17"/>
-      <c r="E54" s="25" t="s">
+      <c r="E54" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25" t="s">
+      <c r="F54" s="24"/>
+      <c r="G54" s="24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="14.4" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="25" t="s">
+      <c r="B55" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="24"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="24" t="s">
         <v>46</v>
       </c>
       <c r="F55" s="40"/>
       <c r="G55" s="40"/>
     </row>
-    <row r="56" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
+    <row r="56" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="24"/>
-      <c r="E56" s="25"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
       <c r="F56" s="15" t="s">
         <v>18</v>
       </c>
@@ -2473,668 +2464,687 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
+    <row r="57" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="C57" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25" t="s">
+      <c r="D57" s="23"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="25" t="s">
+      <c r="G57" s="24" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+    <row r="58" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C58" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="24"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25" t="s">
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G58" s="25" t="s">
+      <c r="G58" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+    <row r="59" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="25" t="s">
+      <c r="C59" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D59" s="24"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25" t="s">
+      <c r="D59" s="23"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="25" t="s">
+      <c r="G59" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+    <row r="60" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25" t="s">
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="G60" s="25" t="s">
+      <c r="G60" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
+    <row r="61" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="25" t="s">
+      <c r="B61" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="D61" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="E61" s="25" t="s">
+      <c r="D61" s="26"/>
+      <c r="E61" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="F61" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="G61" s="25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="26.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="G61" s="24" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="26.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C62" s="25"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="25" t="s">
+      <c r="C62" s="24"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="24" t="s">
         <v>157</v>
       </c>
       <c r="F62" s="40"/>
       <c r="G62" s="40"/>
     </row>
-    <row r="63" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+    <row r="63" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C63" s="25" t="s">
+      <c r="C63" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="24"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25" t="s">
+      <c r="D63" s="23"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G63" s="25" t="s">
+      <c r="G63" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
+    <row r="64" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B64" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25" t="s">
+      <c r="D64" s="23"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G64" s="25" t="s">
+      <c r="G64" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
+    <row r="65" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25" t="s">
+      <c r="D65" s="23"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G66" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" s="23"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G67" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" s="23"/>
+      <c r="E68" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" s="26"/>
+      <c r="E70" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D71" s="26"/>
+      <c r="E71" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="G71" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D72" s="26"/>
+      <c r="E72" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="F72" s="24" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
+      <c r="G72" s="24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" s="24"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="G66" s="25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="s">
+      <c r="B73" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="G73" s="24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C67" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D67" s="24"/>
-      <c r="E67" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
+      <c r="B74" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" s="23"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G74" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" s="24"/>
-      <c r="E68" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="G68" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="s">
+      <c r="B75" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G75" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C69" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F69" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G69" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="24" t="s">
+      <c r="B76" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D76" s="23"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B70" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="D70" s="27"/>
-      <c r="E70" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="F70" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="G70" s="25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
+      <c r="B77" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" s="23"/>
+      <c r="E77" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G77" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C71" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="F71" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="G71" s="25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="24" t="s">
+      <c r="B78" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="23"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="F72" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="G72" s="25" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="24" t="s">
+      <c r="B79" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G79" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C73" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D73" s="24"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G73" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
+      <c r="B80" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D80" s="23"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B74" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C74" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D74" s="24"/>
-      <c r="E74" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F74" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G74" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
+      <c r="B81" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" s="23"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G81" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D75" s="24"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="24" t="s">
+      <c r="B82" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D82" s="23"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G82" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C76" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="24"/>
-      <c r="E76" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F76" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="G76" s="25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="24" t="s">
+      <c r="B83" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D83" s="23"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G83" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B77" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C77" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D77" s="24"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="24" t="s">
+      <c r="B84" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D84" s="23"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G84" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="24"/>
-      <c r="E78" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F78" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G78" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="24" t="s">
+      <c r="B85" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" s="23"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="G85" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D79" s="24"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="G79" s="25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="24" t="s">
+      <c r="B86" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D86" s="23"/>
+      <c r="E86" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D80" s="24"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G80" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="24" t="s">
+      <c r="B87" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D87" s="23"/>
+      <c r="E87" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="G87" s="24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C81" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D81" s="24"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G81" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C82" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D82" s="24"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="G82" s="25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D83" s="24"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G83" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C84" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="D84" s="24"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="G84" s="25" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C85" s="25" t="s">
+      <c r="B88" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C88" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="D85" s="24"/>
-      <c r="E85" s="25" t="s">
+      <c r="D88" s="23"/>
+      <c r="E88" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="F85" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="G85" s="25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C86" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="D86" s="24"/>
-      <c r="E86" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="F86" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="G86" s="25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C87" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="D87" s="24"/>
-      <c r="E87" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="F87" s="25" t="s">
+      <c r="F88" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="G87" s="25" t="s">
+      <c r="G88" s="24" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
+    <row r="89" spans="1:7" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B88" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
-      <c r="F88" s="39"/>
-      <c r="G88" s="39"/>
-    </row>
-    <row r="89" spans="1:7" s="21" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="24" t="s">
+      <c r="B89" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="39"/>
+    </row>
+    <row r="90" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B89" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C89" s="25" t="s">
+      <c r="B90" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C90" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D89" s="24"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25" t="s">
+      <c r="D90" s="23"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G89" s="25" t="s">
+      <c r="G90" s="24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="21" customFormat="1" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="24" t="s">
+    <row r="91" spans="1:7" s="20" customFormat="1" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C90" s="25" t="s">
+      <c r="B91" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D90" s="24"/>
-      <c r="E90" s="25" t="s">
+      <c r="D91" s="23"/>
+      <c r="E91" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="F90" s="25" t="s">
+      <c r="F91" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="G90" s="25" t="s">
+      <c r="G91" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:7" collapsed="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:7" collapsed="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="C89:G89"/>
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="A43:G43"/>
@@ -3158,7 +3168,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B45:B90 B5:B42</xm:sqref>
+          <xm:sqref>B45:B91 B5:B42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3174,9 +3184,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Testplan um Import erweitert
</commit_message>
<xml_diff>
--- a/Testplan.xlsx
+++ b/Testplan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="268">
   <si>
     <t>Testplan</t>
   </si>
@@ -743,21 +748,12 @@
     <t>Mit der Maus auf einen Vorgarten eines Gebäudes klicken</t>
   </si>
   <si>
-    <t>Je nach Auswahl von Straßen oder Regenbögen entstehen zwischen dem ausgewählten Gebäude und allen anderen Gebäude Straßen/Regenbögen</t>
-  </si>
-  <si>
     <t>Verbindungen werden aktiviert und es kann die Darstellungsweise entschieden werden</t>
   </si>
   <si>
     <t>Verbindungsart wählen</t>
   </si>
   <si>
-    <t>Entweder die Checkbox "Regenbögen" oder "Straßen" anklicken, "Änderungen speichern" klicken</t>
-  </si>
-  <si>
-    <t>Je nach Wahl, werden in der Stadtansicht die Verbindungen als Straßen oder als Regenbögen dargestellt</t>
-  </si>
-  <si>
     <t>Attributnamenänderung</t>
   </si>
   <si>
@@ -768,13 +764,97 @@
   </si>
   <si>
     <t>Der Attributname kann beliebig angepasst werden, speichern ist nicht möglich, nur mit der aktuellen Ansicht URL exportiertbar</t>
+  </si>
+  <si>
+    <t>Datensatz importieren</t>
+  </si>
+  <si>
+    <t>Man befindet sich auf der Startseite</t>
+  </si>
+  <si>
+    <t>Auf "CSV Datei importieren" klicken</t>
+  </si>
+  <si>
+    <t>Datensatz auswählen</t>
+  </si>
+  <si>
+    <t>Unter "CSV Datei" auf "Durchsuchen" klicken</t>
+  </si>
+  <si>
+    <t>Man befindet sich auf der Importseite und es befindet sich eine CSV Datei lokal auf dem Rechner</t>
+  </si>
+  <si>
+    <t>Es erscheint Windows Explorer zum Auswählen der CSV Datei</t>
+  </si>
+  <si>
+    <t>Zur gewünschten CSV Datei navigieren und auf "Öffnen" klicken</t>
+  </si>
+  <si>
+    <t>Der Dateiname steht nun neben dem Button "Durchsuchen"</t>
+  </si>
+  <si>
+    <t>Name der Datei</t>
+  </si>
+  <si>
+    <t>Datei ausgewählt</t>
+  </si>
+  <si>
+    <t>Auf "Name der Collection nutzen" klicken</t>
+  </si>
+  <si>
+    <t>Der Datensatz bekommt beim Importieren den Namen durch die Datei vorgegeben</t>
+  </si>
+  <si>
+    <t>Auf "Name eingeben" klicken und einen gewünschten Namen eingeben</t>
+  </si>
+  <si>
+    <t>Der Datensatz bekommt beim Importieren den angegebenen Namen</t>
+  </si>
+  <si>
+    <t>Verbindungen auswählen</t>
+  </si>
+  <si>
+    <t>Unter "Verbindungen" auf "Durchsuchen" klicken</t>
+  </si>
+  <si>
+    <t>Es erscheint Windows Explorer zum Auswählen der Verbindungsdatei</t>
+  </si>
+  <si>
+    <t>Zur gewünschten Verbindungsdatei navigieren und auf "Öffnen" klicken</t>
+  </si>
+  <si>
+    <t>Entweder die Checkbox "Bögen" oder "Straßen" anklicken, "Änderungen speichern" klicken</t>
+  </si>
+  <si>
+    <t>Je nach Wahl, werden in der Stadtansicht die Verbindungen als Straßen oder als Bögen dargestellt</t>
+  </si>
+  <si>
+    <t>Je nach Auswahl von Straßen oder Bögen entstehen zwischen dem ausgewählten Gebäude und allen anderen Gebäude Straßen/Bögen</t>
+  </si>
+  <si>
+    <t>Auf "Import starten" klicken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Import wird durchgeführt und eine Ladeanzeige zeigt den aktuellen Importstatus an. </t>
+  </si>
+  <si>
+    <t>Import 100%</t>
+  </si>
+  <si>
+    <t>Auf "Zum Datensatz" klicken</t>
+  </si>
+  <si>
+    <t>Es wird auf die Seite der Ansichten dieses Datensatzes weitergeleitet</t>
+  </si>
+  <si>
+    <t>Es wird auf die Seite zum Importieren weiter geleitet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +969,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -975,7 +1061,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1037,44 +1123,56 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1087,10 +1185,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1367,7 +1465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1375,39 +1473,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V92"/>
+  <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B98" sqref="B98"/>
+      <selection pane="bottomRight" activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="80.33203125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="6.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="10"/>
+    <col min="1" max="1" width="20.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="80.28515625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="9"/>
@@ -1416,7 +1514,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:22" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1426,87 +1524,87 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-    </row>
-    <row r="5" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="1:22" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="37" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="24" t="s">
+      <c r="F6" s="42"/>
+      <c r="G6" s="33" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1625,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
@@ -1537,7 +1635,7 @@
       <c r="C8" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="15" t="s">
         <v>91</v>
       </c>
@@ -1548,17 +1646,17 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="15" t="s">
         <v>91</v>
       </c>
@@ -1569,18 +1667,18 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="24" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="33" t="s">
         <v>108</v>
       </c>
       <c r="F10" s="17" t="s">
@@ -1590,18 +1688,18 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="33" t="s">
         <v>108</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -1611,1553 +1709,1747 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="11" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:22" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="1:22" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="B22" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+    </row>
+    <row r="23" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="B23" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="24" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F23" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G23" s="33" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+    <row r="24" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="B24" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24" t="s">
+      <c r="D24" s="33"/>
+      <c r="E24" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F24" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G24" s="33" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+    <row r="25" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B25" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="24" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F25" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G25" s="33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:22" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+    <row r="26" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B26" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="24" t="s">
+      <c r="D26" s="25"/>
+      <c r="E26" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F26" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G26" s="33" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+    <row r="27" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B27" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="24" t="s">
+      <c r="D27" s="25"/>
+      <c r="E27" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F27" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G27" s="33" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+    <row r="28" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="24" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="24" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F28" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G28" s="33" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+    <row r="29" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B29" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="24" t="s">
+      <c r="D29" s="25"/>
+      <c r="E29" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F29" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G29" s="33" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="11" customFormat="1" ht="14.4" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+    <row r="30" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-    </row>
-    <row r="21" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="B30" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+    </row>
+    <row r="31" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="24" t="s">
+      <c r="B31" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="11" customFormat="1" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="23"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="11" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="11" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D35" s="25"/>
+      <c r="E35" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="11" customFormat="1" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37" s="25"/>
+      <c r="E37" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="E38" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="D39" s="25"/>
+      <c r="E39" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="25"/>
+      <c r="E40" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="33"/>
+      <c r="E41" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G41" s="33" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+    <row r="42" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C32" s="24" t="s">
+      <c r="B42" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="17" t="s">
+      <c r="D42" s="33"/>
+      <c r="E42" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F42" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G42" s="33" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+    <row r="43" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C33" s="24" t="s">
+      <c r="B43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="17" t="s">
+      <c r="D43" s="33"/>
+      <c r="E43" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F43" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G43" s="33" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+    <row r="44" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" s="24" t="s">
+      <c r="B44" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="17" t="s">
+      <c r="D44" s="33"/>
+      <c r="E44" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F44" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="G34" s="24" t="s">
+      <c r="G44" s="33" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+    <row r="45" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C35" s="24" t="s">
+      <c r="B45" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="17" t="s">
+      <c r="D45" s="33"/>
+      <c r="E45" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F45" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="G45" s="33" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
+    <row r="46" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C36" s="24" t="s">
+      <c r="B46" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="17" t="s">
+      <c r="D46" s="33"/>
+      <c r="E46" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F46" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G46" s="33" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="11" customFormat="1" ht="27" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
+    <row r="47" spans="1:7" s="11" customFormat="1" ht="27" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="24" t="s">
+      <c r="B47" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="35" t="s">
+      <c r="D47" s="19"/>
+      <c r="E47" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="24" t="s">
+      <c r="F47" s="40"/>
+      <c r="G47" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
+    <row r="48" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" s="24" t="s">
+      <c r="B48" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="17" t="s">
+      <c r="D48" s="33"/>
+      <c r="E48" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F48" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G48" s="33" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="11" customFormat="1" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
+    <row r="49" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="24" t="s">
+      <c r="B49" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="17" t="s">
+      <c r="D49" s="33"/>
+      <c r="E49" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="F49" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G49" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="11" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21" t="s">
+    <row r="50" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-    </row>
-    <row r="41" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22" t="s">
+      <c r="B50" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+    </row>
+    <row r="51" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C41" s="24" t="s">
+      <c r="B51" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24" t="s">
+      <c r="D51" s="33"/>
+      <c r="E51" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="24" t="s">
+      <c r="F51" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G51" s="33" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22" t="s">
+    <row r="52" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="24" t="s">
+      <c r="B52" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="24" t="s">
+      <c r="D52" s="33"/>
+      <c r="E52" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="F42" s="24" t="s">
+      <c r="F52" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G52" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:7" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-    </row>
-    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+    <row r="53" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-    </row>
-    <row r="45" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+    </row>
+    <row r="55" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-    </row>
-    <row r="46" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+      <c r="B55" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+    </row>
+    <row r="56" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" s="24" t="s">
+      <c r="B56" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="24" t="s">
+      <c r="D56" s="22"/>
+      <c r="E56" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F56" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G46" s="24" t="s">
+      <c r="G56" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23" t="s">
+    <row r="57" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="24" t="s">
+      <c r="B57" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15" t="s">
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="23" t="s">
+    <row r="58" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C48" s="24" t="s">
+      <c r="B58" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15" t="s">
+      <c r="D58" s="22"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23" t="s">
+    <row r="59" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C49" s="24" t="s">
+      <c r="B59" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15" t="s">
+      <c r="D59" s="22"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="23" t="s">
+    <row r="60" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C50" s="24" t="s">
+      <c r="B60" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15" t="s">
+      <c r="D60" s="22"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="23" t="s">
+    <row r="61" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C51" s="24" t="s">
+      <c r="B61" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24" t="s">
+      <c r="D61" s="22"/>
+      <c r="E61" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15" t="s">
+      <c r="F61" s="15"/>
+      <c r="G61" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23" t="s">
+    <row r="62" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C52" s="24" t="s">
+      <c r="B62" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15" t="s">
+      <c r="D62" s="22"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="23" t="s">
+    <row r="63" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="17" t="s">
+      <c r="B63" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D53" s="17"/>
-      <c r="E53" s="24" t="s">
+      <c r="D63" s="17"/>
+      <c r="E63" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24" t="s">
+      <c r="F63" s="23"/>
+      <c r="G63" s="23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="23" t="s">
+    <row r="64" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="17" t="s">
+      <c r="B64" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="24" t="s">
+      <c r="D64" s="17"/>
+      <c r="E64" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24" t="s">
+      <c r="F64" s="23"/>
+      <c r="G64" s="23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.4" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="18" t="s">
+    <row r="65" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="24" t="s">
+      <c r="B65" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C65" s="23"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-    </row>
-    <row r="56" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="23" t="s">
+      <c r="F65" s="35"/>
+      <c r="G65" s="35"/>
+    </row>
+    <row r="66" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C56" s="24" t="s">
+      <c r="B66" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="15" t="s">
+      <c r="D66" s="22"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G56" s="15" t="s">
+      <c r="G66" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="23" t="s">
+    <row r="67" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B57" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C57" s="24" t="s">
+      <c r="B67" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="23"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24" t="s">
+      <c r="D67" s="22"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="24" t="s">
+      <c r="G67" s="23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="23" t="s">
+    <row r="68" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C58" s="24" t="s">
+      <c r="B68" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24" t="s">
+      <c r="D68" s="22"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G58" s="24" t="s">
+      <c r="G68" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="23" t="s">
+    <row r="69" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C59" s="24" t="s">
+      <c r="B69" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D59" s="23"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24" t="s">
+      <c r="D69" s="22"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="24" t="s">
+      <c r="G69" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="23" t="s">
+    <row r="70" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C60" s="24" t="s">
+      <c r="B70" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24" t="s">
+      <c r="D70" s="22"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="G60" s="24" t="s">
+      <c r="G70" s="23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="23" t="s">
+    <row r="71" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="24" t="s">
+      <c r="B71" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="D61" s="26"/>
-      <c r="E61" s="24" t="s">
+      <c r="D71" s="25"/>
+      <c r="E71" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F71" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="G61" s="24" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="26.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="18" t="s">
+      <c r="G71" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="26.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C62" s="24"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="24" t="s">
+      <c r="B72" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="23"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
-    </row>
-    <row r="63" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="23" t="s">
+      <c r="F72" s="35"/>
+      <c r="G72" s="35"/>
+    </row>
+    <row r="73" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B63" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C63" s="24" t="s">
+      <c r="B73" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24" t="s">
+      <c r="D73" s="22"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G63" s="24" t="s">
+      <c r="G73" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="23" t="s">
+    <row r="74" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B64" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64" s="24" t="s">
+      <c r="B74" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="23"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24" t="s">
+      <c r="D74" s="22"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G64" s="24" t="s">
+      <c r="G74" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="23" t="s">
+    <row r="75" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C65" s="24" t="s">
+      <c r="B75" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D65" s="23"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24" t="s">
+      <c r="D75" s="22"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="30" t="s">
+    <row r="76" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="30" t="s">
+      <c r="B76" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="G76" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="F66" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="G66" s="30" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="23" t="s">
+    </row>
+    <row r="77" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C67" s="24" t="s">
+      <c r="B77" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D67" s="23"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24" t="s">
+      <c r="D77" s="22"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="G67" s="24" t="s">
+      <c r="G77" s="23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="23" t="s">
+    <row r="78" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" s="24" t="s">
+      <c r="B78" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D68" s="23"/>
-      <c r="E68" s="24" t="s">
+      <c r="D78" s="22"/>
+      <c r="E78" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24" t="s">
+      <c r="F78" s="23"/>
+      <c r="G78" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="23" t="s">
+    <row r="79" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C69" s="24" t="s">
+      <c r="B79" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D69" s="23"/>
-      <c r="E69" s="24" t="s">
+      <c r="D79" s="22"/>
+      <c r="E79" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F69" s="24" t="s">
+      <c r="F79" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="G69" s="24" t="s">
+      <c r="G79" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="23" t="s">
+    <row r="80" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B70" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C70" s="24" t="s">
+      <c r="B80" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C80" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D70" s="26"/>
-      <c r="E70" s="24" t="s">
+      <c r="D80" s="25"/>
+      <c r="E80" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F70" s="24" t="s">
+      <c r="F80" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G70" s="24" t="s">
+      <c r="G80" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="23" t="s">
+    <row r="81" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C71" s="24" t="s">
+      <c r="B81" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C81" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="D71" s="26"/>
-      <c r="E71" s="24" t="s">
+      <c r="D81" s="25"/>
+      <c r="E81" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="F71" s="24" t="s">
+      <c r="F81" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="G71" s="24" t="s">
+      <c r="G81" s="23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="23" t="s">
+    <row r="82" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="24" t="s">
+      <c r="B82" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="D72" s="26"/>
-      <c r="E72" s="24" t="s">
+      <c r="D82" s="25"/>
+      <c r="E82" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="F72" s="24" t="s">
+      <c r="F82" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="G72" s="24" t="s">
+      <c r="G82" s="23" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="23" t="s">
+    <row r="83" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C73" s="24" t="s">
+      <c r="B83" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26" t="s">
+      <c r="D83" s="25"/>
+      <c r="E83" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="F73" s="24" t="s">
+      <c r="F83" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="G73" s="24" t="s">
+      <c r="G83" s="23" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="23" t="s">
+    <row r="84" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B74" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C74" s="24" t="s">
+      <c r="B84" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D74" s="23"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24" t="s">
+      <c r="D84" s="22"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="G74" s="24" t="s">
+      <c r="G84" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="23" t="s">
+    <row r="85" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C75" s="24" t="s">
+      <c r="B85" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D75" s="23"/>
-      <c r="E75" s="24" t="s">
+      <c r="D85" s="22"/>
+      <c r="E85" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F75" s="24" t="s">
+      <c r="F85" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="G75" s="24" t="s">
+      <c r="G85" s="23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="23" t="s">
+    <row r="86" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C76" s="24" t="s">
+      <c r="B86" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C86" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D76" s="23"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24" t="s">
+      <c r="D86" s="22"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="23" t="s">
+    <row r="87" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B77" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C77" s="24" t="s">
+      <c r="B87" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C87" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D77" s="23"/>
-      <c r="E77" s="24" t="s">
+      <c r="D87" s="22"/>
+      <c r="E87" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F77" s="24" t="s">
+      <c r="F87" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G77" s="24" t="s">
+      <c r="G87" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="23" t="s">
+    <row r="88" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="24" t="s">
+      <c r="B88" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C88" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D78" s="23"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24" t="s">
+      <c r="D88" s="22"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="23" t="s">
+    <row r="89" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C79" s="24" t="s">
+      <c r="B89" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D79" s="23"/>
-      <c r="E79" s="24" t="s">
+      <c r="D89" s="22"/>
+      <c r="E89" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F79" s="24" t="s">
+      <c r="F89" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="G79" s="24" t="s">
+      <c r="G89" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="23" t="s">
+    <row r="90" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" s="24" t="s">
+      <c r="B90" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C90" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D80" s="23"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24" t="s">
+      <c r="D90" s="22"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G80" s="24" t="s">
+      <c r="G90" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="23" t="s">
+    <row r="91" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C81" s="24" t="s">
+      <c r="B91" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="23"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24" t="s">
+      <c r="D91" s="22"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G81" s="24" t="s">
+      <c r="G91" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="23" t="s">
+    <row r="92" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C82" s="24" t="s">
+      <c r="B92" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C92" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D82" s="23"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24" t="s">
+      <c r="D92" s="22"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="G82" s="24" t="s">
+      <c r="G92" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
+    <row r="93" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B83" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83" s="24" t="s">
+      <c r="B93" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C93" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D83" s="23"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24" t="s">
+      <c r="D93" s="22"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G83" s="24" t="s">
+      <c r="G93" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="23" t="s">
+    <row r="94" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B84" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C84" s="24" t="s">
+      <c r="B94" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C94" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D84" s="23"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24" t="s">
+      <c r="D94" s="22"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G84" s="24" t="s">
+      <c r="G94" s="23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="23" t="s">
+    <row r="95" spans="1:7" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B85" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C85" s="24" t="s">
+      <c r="B95" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C95" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="D85" s="23"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24" t="s">
+      <c r="D95" s="22"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="G85" s="24" t="s">
+      <c r="G95" s="23" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="23" t="s">
+    <row r="96" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B86" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C86" s="24" t="s">
+      <c r="B96" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C96" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D86" s="23"/>
-      <c r="E86" s="24" t="s">
+      <c r="D96" s="22"/>
+      <c r="E96" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="F86" s="24" t="s">
+      <c r="F96" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G86" s="24" t="s">
+      <c r="G96" s="23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="23" t="s">
+    <row r="97" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C87" s="24" t="s">
+      <c r="B97" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C97" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="D87" s="23"/>
-      <c r="E87" s="24" t="s">
+      <c r="D97" s="22"/>
+      <c r="E97" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="F87" s="24" t="s">
+      <c r="F97" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="G87" s="24" t="s">
+      <c r="G97" s="23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="23" t="s">
+    <row r="98" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B88" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C88" s="24" t="s">
+      <c r="B98" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C98" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D88" s="23"/>
-      <c r="E88" s="24" t="s">
+      <c r="D98" s="22"/>
+      <c r="E98" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="F88" s="24" t="s">
+      <c r="F98" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="G88" s="24" t="s">
+      <c r="G98" s="23" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="89" spans="1:7" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="18" t="s">
+    <row r="99" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B89" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
-      <c r="G89" s="39"/>
-    </row>
-    <row r="90" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="23" t="s">
+      <c r="B99" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="34"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="34"/>
+      <c r="F99" s="34"/>
+      <c r="G99" s="34"/>
+    </row>
+    <row r="100" spans="1:7" s="20" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C90" s="24" t="s">
+      <c r="B100" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C100" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D90" s="23"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24" t="s">
+      <c r="D100" s="22"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G90" s="24" t="s">
+      <c r="G100" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="20" customFormat="1" ht="45.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="23" t="s">
+    <row r="101" spans="1:7" s="20" customFormat="1" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C91" s="24" t="s">
+      <c r="B101" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C101" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D91" s="23"/>
-      <c r="E91" s="24" t="s">
+      <c r="D101" s="22"/>
+      <c r="E101" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="F91" s="24" t="s">
+      <c r="F101" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G91" s="24" t="s">
+      <c r="G101" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:7" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:7" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="A44:G44"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C50:G50"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A54:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3168,7 +3460,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B45:B91 B5:B42</xm:sqref>
+          <xm:sqref>B55:B101 B5:B52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3184,9 +3476,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Testplan aktualisiert, Alle Tests erneut mit IE getestet
</commit_message>
<xml_diff>
--- a/Testplan.xlsx
+++ b/Testplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="338">
   <si>
     <t>Testplan</t>
   </si>
@@ -163,9 +163,6 @@
     <t>eine Stadt ist zu sehen</t>
   </si>
   <si>
-    <t>Auf "Close Menu" klicken</t>
-  </si>
-  <si>
     <t>Menü wird ausgeblendet</t>
   </si>
   <si>
@@ -385,9 +382,6 @@
     <t>Auf "Dimensionen der Gebäude definieren" klicken</t>
   </si>
   <si>
-    <t>Die Dimensionen Name, Fläche, Höhe, Farbe erscheinen</t>
-  </si>
-  <si>
     <t>Dimensionen sind offen</t>
   </si>
   <si>
@@ -457,9 +451,6 @@
     <t>Unter "Feld" eine der Attribute wählen</t>
   </si>
   <si>
-    <t>Blöcke wählen</t>
-  </si>
-  <si>
     <t>Blöcke hinzufügen</t>
   </si>
   <si>
@@ -580,9 +571,6 @@
     <t>Es erscheint eine Fehlermeldung, die besagt, dass keine Blöcke ausgewählt wurden</t>
   </si>
   <si>
-    <t>Jedes Gebäude und jedes Distrikt, das Verbindungen hat, hat zwei Vorgärten in Form von Pfeilen</t>
-  </si>
-  <si>
     <t>Datensätze</t>
   </si>
   <si>
@@ -680,9 +668,6 @@
   </si>
   <si>
     <t>Es kann über "Summe, Durchschnitt, Erster Wert, Letzter Wert, Maximum, Minimum, Standardabweichung" aggregiert werden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nach aktualisieren der Stadtansicht wird die Blockbildung angewendet aufgrund des ausgewählten Attributs  </t>
   </si>
   <si>
     <t>Dimensionen wurden den richtigen Werten zugeordnet (zu vergleichen mit den Werten unter der Ansicht)</t>
@@ -764,9 +749,6 @@
     <t>Datei ausgewählt</t>
   </si>
   <si>
-    <t>Auf "Name der Collection nutzen" klicken</t>
-  </si>
-  <si>
     <t>Der Datensatz bekommt beim Importieren den Namen durch die Datei vorgegeben</t>
   </si>
   <si>
@@ -786,9 +768,6 @@
   </si>
   <si>
     <t>Zur gewünschten Verbindungsdatei navigieren und auf "Öffnen" klicken</t>
-  </si>
-  <si>
-    <t>Entweder die Checkbox "Bögen" oder "Straßen" anklicken, "Änderungen speichern" klicken</t>
   </si>
   <si>
     <t>Je nach Wahl, werden in der Stadtansicht die Verbindungen als Straßen oder als Bögen dargestellt</t>
@@ -913,9 +892,6 @@
     <t>Wird als Buchstabe intepretiert, je nach Stelle treten einer der 3 obigen Fälle ein. Das Sonderzeichen wird als "?" wiedergegeben</t>
   </si>
   <si>
-    <t>Gebäude mit Verbindungen</t>
-  </si>
-  <si>
     <t>Checkbox "Gebäude mit Verbindungen" aktivieren</t>
   </si>
   <si>
@@ -979,13 +955,106 @@
     <t>Man kehrt in die Datensatzübersicht zurück</t>
   </si>
   <si>
-    <t>DataCity mit einem Browser geöffnet, der WebGl kann</t>
-  </si>
-  <si>
     <t>Eine Stadt anzeigen lassen, welche mehr als 100.000 Gebäude anzeigen soll</t>
   </si>
   <si>
     <t>Je nach Browser kommt es zu einer Fehlermeldung, dass das Skript stehen geblieben ist oder die Stadt wird nach langem Laden nicht angezeigt. DataCity ist für eine Ansicht von 100.000 Gebäude ausgelegt. Darüber kann es zu Ladeproblemen kommen</t>
+  </si>
+  <si>
+    <t>Auf "Name der CSV-Datei nutzen" klicken</t>
+  </si>
+  <si>
+    <t>Ansicht verwalten</t>
+  </si>
+  <si>
+    <t>Auf "Experimentelle Version anschalten" klicken</t>
+  </si>
+  <si>
+    <t>Es werden weitere Funktionalitäten für die Stadtansicht freigeschaltet, Achtung: Funktionalitäten sind nicht bugfrei. Es kann zu fehlerhaften Darstellungen kommen</t>
+  </si>
+  <si>
+    <t>Blöcke auswählen</t>
+  </si>
+  <si>
+    <t>PunktBlockbildung</t>
+  </si>
+  <si>
+    <t>Klicken auf "Es wird nach jedem Punkt eine neue Ebene gebildet"</t>
+  </si>
+  <si>
+    <t>Durch diese Auswahl werden Blöcke abhängig vom Packagenamen gebildet. Nach jedem Punkt im Packagename entsteht ein neuer Block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nach dem Aktualisieren der Stadtansicht wird die Blockbildung angewendet aufgrund des ausgewählten Attributs  </t>
+  </si>
+  <si>
+    <t>"4.Blöcke definieren" wurde geöffnet</t>
+  </si>
+  <si>
+    <t>Die Dimensionen ID, Fläche, Höhe, Farbe erscheinen</t>
+  </si>
+  <si>
+    <t>Dimensionen logarithmieren</t>
+  </si>
+  <si>
+    <t>Klicken auf die Checkbox unter "logarithmieren"</t>
+  </si>
+  <si>
+    <t>Die Dimensionen werden noch vor der Stadtansicht logarithmiert. Das Logarithmieren kann auch direkt in der Stadtansicht erneut angepasst werden.</t>
+  </si>
+  <si>
+    <t>Für die Dimensionen wurden Attribute ausgewählt</t>
+  </si>
+  <si>
+    <t>Jedes Gebäude und jedes Distrikt, das Verbindungen hat, hat zwei Vorgärten in Form von Pfeilen (wenn diese eingeschaltet wurden [Exp</t>
+  </si>
+  <si>
+    <t>Entweder die Checkbox "Bögen" oder "Straßen" anklicken (Achtung: Bögen und Straßen nur in der Experimentellen Version auswählbar)</t>
+  </si>
+  <si>
+    <t>Vorgärten zeichnen</t>
+  </si>
+  <si>
+    <t>"Verbindungen nutzen" wurde ausgewählt</t>
+  </si>
+  <si>
+    <t>Klicken auf die Checkbox "Vorgärten nutzen"</t>
+  </si>
+  <si>
+    <t>Die Vorgärten werden in der Stadtdarstellung vor jedem Gebäude mit Verbindungen dargestellt</t>
+  </si>
+  <si>
+    <t>DataCity mit einem Browser geöffnet, der WebGl unterstützt</t>
+  </si>
+  <si>
+    <t>Pfeiltasten</t>
+  </si>
+  <si>
+    <t>Pfeiltasten drücken</t>
+  </si>
+  <si>
+    <t>Das Sichtfeld bewegt sich in die gedrückte Pfeiltastenrichtung</t>
+  </si>
+  <si>
+    <t>Auf "Close Controls" klicken</t>
+  </si>
+  <si>
+    <t>Gebäude mit Verbindungen (Es muss eine Verbindungs CSV zuvor mit importiert worden sein)</t>
+  </si>
+  <si>
+    <t>Menü (experimentelle Version)</t>
+  </si>
+  <si>
+    <t>Ansicht bearbeiten (experimentelle Version)</t>
+  </si>
+  <si>
+    <t>Man hat ein Gebäude durch die Gebäudesuche fixiert</t>
+  </si>
+  <si>
+    <t>Klicken auf "Auswahl deaktivieren"</t>
+  </si>
+  <si>
+    <t>Das fixierte Gebäude, welches durch die Gebäudesuche gefunden wurde, wird wieder deaktiviert</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1273,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1313,6 +1382,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1337,29 +1433,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1635,7 +1716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1643,13 +1724,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V116"/>
+  <dimension ref="A1:V122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B115" sqref="B115"/>
+      <selection pane="bottomRight" activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1666,16 +1747,16 @@
     <col min="23" max="16384" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="9"/>
@@ -1684,12 +1765,12 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:22" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="8"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1732,46 +1813,46 @@
       <c r="V3" s="28"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="A4" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
+        <v>152</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D6" s="32"/>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="46"/>
+      <c r="G6" s="33" t="s">
         <v>188</v>
-      </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="33" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1779,20 +1860,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>92</v>
-      </c>
       <c r="G7" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1800,20 +1881,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1821,20 +1902,20 @@
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1842,20 +1923,20 @@
         <v>6</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1863,28 +1944,28 @@
         <v>6</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>38</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="25"/>
@@ -1894,375 +1975,375 @@
     </row>
     <row r="13" spans="1:22" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="25"/>
       <c r="E13" s="33" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="33" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="33"/>
       <c r="F15" s="17" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="33" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>241</v>
+        <v>306</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="33" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>246</v>
-      </c>
       <c r="G18" s="17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="33"/>
       <c r="F19" s="17" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="33" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="25"/>
       <c r="E21" s="33" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>258</v>
+      <c r="A22" s="35" t="s">
+        <v>251</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E22" s="34"/>
       <c r="F22" s="17" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="34"/>
       <c r="F23" s="17" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="34"/>
       <c r="F24" s="17" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25" s="34"/>
       <c r="F25" s="17" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="34"/>
       <c r="F26" s="17" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="34"/>
       <c r="F27" s="17" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="34"/>
       <c r="F28" s="17" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="34"/>
       <c r="F29" s="17" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="34"/>
       <c r="F30" s="17" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="34"/>
       <c r="F31" s="17" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -2270,20 +2351,20 @@
         <v>9</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
+        <v>152</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
     </row>
     <row r="33" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>33</v>
@@ -2296,7 +2377,7 @@
         <v>35</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2304,20 +2385,20 @@
         <v>9</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C34" s="33" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="33" t="s">
-        <v>95</v>
-      </c>
       <c r="G34" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2325,20 +2406,20 @@
         <v>9</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D35" s="37"/>
       <c r="E35" s="37" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2346,7 +2427,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>11</v>
@@ -2356,10 +2437,10 @@
         <v>40</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2367,20 +2448,20 @@
         <v>9</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F37" s="33" t="s">
         <v>37</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2388,20 +2469,20 @@
         <v>9</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F38" s="33" t="s">
         <v>38</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2410,17 +2491,17 @@
       </c>
       <c r="B39" s="16"/>
       <c r="C39" s="33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="F39" s="33" t="s">
-        <v>180</v>
-      </c>
       <c r="G39" s="33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2428,645 +2509,653 @@
         <v>9</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G40" s="33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="G41" s="39" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+    </row>
+    <row r="43" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="33"/>
+      <c r="E43" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-    </row>
-    <row r="42" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="33" t="s">
+      <c r="G43" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F43" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="G43" s="33" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="17" t="s">
-        <v>183</v>
+        <v>115</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="G44" s="33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="17" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="G45" s="33" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>203</v>
+        <v>134</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="17" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F46" s="33" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="G46" s="33" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A47" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="17" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F47" s="33" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="36" t="s">
-        <v>113</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="11" customFormat="1" ht="57" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="32" t="s">
+        <v>334</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C48" s="37" t="s">
-        <v>306</v>
+        <v>152</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>220</v>
       </c>
       <c r="D48" s="25"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="37" t="s">
-        <v>307</v>
-      </c>
-      <c r="G48" s="37" t="s">
-        <v>308</v>
+      <c r="E48" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
-        <v>113</v>
+      <c r="A49" s="38" t="s">
+        <v>112</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C49" s="33" t="s">
-        <v>209</v>
+        <v>152</v>
+      </c>
+      <c r="C49" s="39" t="s">
+        <v>323</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="F49" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="32" t="s">
-        <v>113</v>
+        <v>324</v>
+      </c>
+      <c r="F49" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="G49" s="39" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C50" s="33" t="s">
-        <v>207</v>
+        <v>152</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>298</v>
       </c>
       <c r="D50" s="25"/>
-      <c r="E50" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="F50" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="G50" s="33" t="s">
-        <v>214</v>
+      <c r="E50" s="17"/>
+      <c r="F50" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="G50" s="37" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="17" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="F51" s="33" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="17" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" s="33"/>
+        <v>203</v>
+      </c>
+      <c r="D53" s="25"/>
       <c r="E53" s="17" t="s">
-        <v>40</v>
+        <v>212</v>
       </c>
       <c r="F53" s="33" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="D54" s="33"/>
+        <v>203</v>
+      </c>
+      <c r="D54" s="25"/>
       <c r="E54" s="17" t="s">
-        <v>140</v>
+        <v>213</v>
       </c>
       <c r="F54" s="33" t="s">
-        <v>141</v>
+        <v>214</v>
       </c>
       <c r="G54" s="33" t="s">
-        <v>142</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A55" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C55" s="33" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="D55" s="33"/>
       <c r="E55" s="17" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="F55" s="33" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G55" s="33" t="s">
-        <v>220</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="32" t="s">
-        <v>113</v>
+      <c r="A56" s="38" t="s">
+        <v>112</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="D56" s="33"/>
+        <v>152</v>
+      </c>
+      <c r="C56" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="D56" s="39"/>
       <c r="E56" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="F56" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="G56" s="33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+      <c r="F56" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A57" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>119</v>
+        <v>310</v>
       </c>
       <c r="D57" s="33"/>
       <c r="E57" s="17" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="F57" s="33" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A58" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="D58" s="33"/>
       <c r="E58" s="17" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="F58" s="33" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="11" customFormat="1" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A59" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="D59" s="19"/>
-      <c r="E59" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="F59" s="50"/>
+        <v>156</v>
+      </c>
+      <c r="D59" s="33"/>
+      <c r="E59" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F59" s="33" t="s">
+        <v>158</v>
+      </c>
       <c r="G59" s="33" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A60" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D60" s="33"/>
       <c r="E60" s="17" t="s">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="F60" s="33" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>158</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A61" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D61" s="33"/>
       <c r="E61" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F61" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G61" s="33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="D62" s="56"/>
+      <c r="E62" s="57" t="s">
+        <v>320</v>
+      </c>
+      <c r="F62" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="G62" s="39" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="11" customFormat="1" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="19"/>
+      <c r="E63" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" s="44"/>
+      <c r="G63" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="33"/>
+      <c r="E64" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F64" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G64" s="33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="33"/>
+      <c r="E65" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="G65" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+    </row>
+    <row r="67" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F67" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G67" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G68" s="33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="14.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="50"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="52"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="G61" s="33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="46"/>
-    </row>
-    <row r="63" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C63" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G63" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="F64" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G64" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="14.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="41"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="43"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="40"/>
-    </row>
-    <row r="67" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="21" t="s">
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="48"/>
+      <c r="G70" s="49"/>
+    </row>
+    <row r="71" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C67" s="46"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="46"/>
-    </row>
-    <row r="68" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="22"/>
-      <c r="E68" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F68" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="22"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C70" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="22"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="B71" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="40"/>
     </row>
     <row r="72" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C72" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D72" s="22"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="E72" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A73" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C73" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D73" s="22"/>
-      <c r="E73" s="23" t="s">
-        <v>163</v>
-      </c>
+      <c r="E73" s="23"/>
       <c r="F73" s="15"/>
       <c r="G73" s="15" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3074,7 +3163,7 @@
         <v>45</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C74" s="23" t="s">
         <v>14</v>
@@ -3083,26 +3172,24 @@
       <c r="E74" s="23"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A75" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" s="17"/>
-      <c r="E75" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="F75" s="23"/>
-      <c r="G75" s="23" t="s">
-        <v>77</v>
+        <v>152</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="22"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3110,632 +3197,628 @@
         <v>45</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D76" s="17"/>
-      <c r="E76" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="23"/>
+        <v>152</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="22"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="D77" s="22"/>
       <c r="E77" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-    </row>
-    <row r="78" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A78" s="22" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="F78" s="15"/>
       <c r="G78" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A79" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="17"/>
+      <c r="E79" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D80" s="17"/>
+      <c r="E80" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" s="22"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G79" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D80" s="22"/>
-      <c r="E80" s="23"/>
-      <c r="F80" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G80" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" s="23" t="s">
-        <v>24</v>
-      </c>
+      <c r="B81" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="23"/>
       <c r="D81" s="22"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G81" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="E81" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" s="54"/>
+      <c r="G81" s="54"/>
     </row>
     <row r="82" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A82" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="G82" s="23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F82" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A83" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="30" t="s">
-        <v>155</v>
+      <c r="B83" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="D83" s="25"/>
-      <c r="E83" s="23" t="s">
-        <v>174</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D83" s="22"/>
+      <c r="E83" s="23"/>
       <c r="F83" s="23" t="s">
-        <v>223</v>
+        <v>21</v>
       </c>
       <c r="G83" s="23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="23"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="D84" s="22"/>
-      <c r="E84" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="F84" s="45"/>
-      <c r="G84" s="45"/>
-    </row>
-    <row r="85" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="E84" s="23"/>
+      <c r="F84" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A85" s="22" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="23"/>
       <c r="F85" s="23" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="G85" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A86" s="22" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="23"/>
       <c r="F86" s="23" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="G86" s="23" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="22" t="s">
+      <c r="A87" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C87" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="G87" s="39" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D88" s="25"/>
+      <c r="E88" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F88" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="G88" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C87" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D87" s="22"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="23" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C88" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="D88" s="29"/>
-      <c r="E88" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="F88" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="G88" s="29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C89" s="23" t="s">
-        <v>29</v>
-      </c>
+      <c r="B89" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C89" s="23"/>
       <c r="D89" s="22"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="G89" s="23" t="s">
+      <c r="E89" s="23" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F89" s="54"/>
+      <c r="G89" s="54"/>
+    </row>
+    <row r="90" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A90" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D90" s="22"/>
-      <c r="E90" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23" t="s">
+        <v>331</v>
+      </c>
       <c r="G90" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D91" s="22"/>
-      <c r="E91" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="E91" s="23"/>
       <c r="F91" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G91" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D92" s="25"/>
-      <c r="E92" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F92" s="23" t="s">
-        <v>54</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D92" s="22"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
       <c r="G92" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C93" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="D93" s="25"/>
-      <c r="E93" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="F93" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="G93" s="23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="C93" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="F93" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="G93" s="29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A94" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="D94" s="25"/>
-      <c r="E94" s="23" t="s">
-        <v>295</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D94" s="22"/>
+      <c r="E94" s="23"/>
       <c r="F94" s="23" t="s">
-        <v>294</v>
+        <v>48</v>
       </c>
       <c r="G94" s="23" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A95" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>297</v>
-      </c>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F95" s="23" t="s">
-        <v>298</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D95" s="22"/>
+      <c r="E95" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F95" s="23"/>
       <c r="G95" s="23" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A96" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C96" s="23" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D96" s="22"/>
-      <c r="E96" s="23"/>
+      <c r="E96" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="F96" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G96" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A97" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D97" s="22"/>
+        <v>29</v>
+      </c>
+      <c r="D97" s="25"/>
       <c r="E97" s="23" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="F97" s="23" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G97" s="23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="57" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A98" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D98" s="22"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="23"/>
+        <v>332</v>
+      </c>
+      <c r="D98" s="25"/>
+      <c r="E98" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F98" s="23" t="s">
+        <v>283</v>
+      </c>
       <c r="G98" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A99" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D99" s="22"/>
+        <v>285</v>
+      </c>
+      <c r="D99" s="25"/>
       <c r="E99" s="23" t="s">
-        <v>98</v>
+        <v>287</v>
       </c>
       <c r="F99" s="23" t="s">
-        <v>61</v>
+        <v>286</v>
       </c>
       <c r="G99" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A100" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D100" s="22"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="23"/>
+        <v>289</v>
+      </c>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="F100" s="23" t="s">
+        <v>290</v>
+      </c>
       <c r="G100" s="23" t="s">
-        <v>103</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A101" s="22" t="s">
-        <v>26</v>
+        <v>333</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C101" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D101" s="22"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D101" s="22"/>
-      <c r="E101" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F101" s="23" t="s">
-        <v>62</v>
-      </c>
       <c r="G101" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A102" s="22" t="s">
-        <v>26</v>
+        <v>333</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D102" s="22"/>
-      <c r="E102" s="23"/>
+      <c r="E102" s="23" t="s">
+        <v>97</v>
+      </c>
       <c r="F102" s="23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G102" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A103" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D103" s="22"/>
       <c r="E103" s="23"/>
-      <c r="F103" s="23" t="s">
-        <v>67</v>
-      </c>
+      <c r="F103" s="23"/>
       <c r="G103" s="23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A104" s="22" t="s">
-        <v>26</v>
+        <v>333</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D104" s="22"/>
-      <c r="E104" s="23"/>
+      <c r="E104" s="23" t="s">
+        <v>97</v>
+      </c>
       <c r="F104" s="23" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G104" s="23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A105" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D105" s="22"/>
       <c r="E105" s="23"/>
-      <c r="F105" s="23" t="s">
-        <v>71</v>
-      </c>
+      <c r="F105" s="23"/>
       <c r="G105" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A106" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C106" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D106" s="22"/>
+      <c r="E106" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F106" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G106" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B106" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" s="23" t="s">
+      <c r="B107" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C107" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D107" s="22"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D106" s="22"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G106" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B107" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C107" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D107" s="37"/>
-      <c r="E107" s="37"/>
-      <c r="F107" s="37" t="s">
-        <v>300</v>
-      </c>
-      <c r="G107" s="37" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="G107" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A108" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>164</v>
+        <v>63</v>
       </c>
       <c r="D108" s="22"/>
       <c r="E108" s="23"/>
       <c r="F108" s="23" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
       <c r="G108" s="23" t="s">
-        <v>191</v>
+        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3743,41 +3826,37 @@
         <v>26</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>169</v>
+        <v>63</v>
       </c>
       <c r="D109" s="22"/>
-      <c r="E109" s="23" t="s">
-        <v>168</v>
-      </c>
+      <c r="E109" s="23"/>
       <c r="F109" s="23" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="G109" s="23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A110" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>165</v>
+        <v>63</v>
       </c>
       <c r="D110" s="22"/>
-      <c r="E110" s="23" t="s">
-        <v>168</v>
-      </c>
+      <c r="E110" s="23"/>
       <c r="F110" s="23" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="G110" s="23" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3785,129 +3864,249 @@
         <v>26</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>169</v>
+        <v>63</v>
       </c>
       <c r="D111" s="22"/>
-      <c r="E111" s="23" t="s">
-        <v>168</v>
-      </c>
+      <c r="E111" s="23"/>
       <c r="F111" s="23" t="s">
-        <v>172</v>
+        <v>72</v>
       </c>
       <c r="G111" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B112" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C112" s="44"/>
-      <c r="D112" s="44"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="44"/>
-      <c r="G112" s="44"/>
-    </row>
-    <row r="113" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C112" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D112" s="37"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="37" t="s">
+        <v>292</v>
+      </c>
+      <c r="G112" s="37" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A113" s="22" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="D113" s="22"/>
       <c r="E113" s="23"/>
       <c r="F113" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G113" s="23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C114" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="D114" s="39"/>
+      <c r="E114" s="39" t="s">
+        <v>335</v>
+      </c>
+      <c r="F114" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="G114" s="39" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C115" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" s="22"/>
+      <c r="E115" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F115" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="G115" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D116" s="22"/>
+      <c r="E116" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F116" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G116" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C117" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D117" s="22"/>
+      <c r="E117" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F117" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G117" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C118" s="53"/>
+      <c r="D118" s="53"/>
+      <c r="E118" s="53"/>
+      <c r="F118" s="53"/>
+      <c r="G118" s="53"/>
+    </row>
+    <row r="119" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C119" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D119" s="22"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G113" s="23" t="s">
+      <c r="G119" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="20" customFormat="1" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C120" s="23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" s="20" customFormat="1" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B114" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C114" s="23" t="s">
+      <c r="D120" s="22"/>
+      <c r="E120" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D114" s="22"/>
-      <c r="E114" s="23" t="s">
+      <c r="F120" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="F114" s="23" t="s">
+      <c r="G120" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G114" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B115" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C115" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D115" s="37"/>
-      <c r="E115" s="37" t="s">
-        <v>312</v>
-      </c>
-      <c r="F115" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="G115" s="37" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B116" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="C116" s="37" t="s">
-        <v>309</v>
-      </c>
-      <c r="F116" s="37" t="s">
-        <v>310</v>
-      </c>
-      <c r="G116" s="37" t="s">
-        <v>311</v>
+    </row>
+    <row r="121" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C121" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D121" s="37"/>
+      <c r="E121" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="F121" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="G121" s="37" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A122" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C122" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="F122" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="G122" s="37" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="C71:G71"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C66:G66"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="E63:F63"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="C67:G67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3918,7 +4117,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B67:B115 B5:B64</xm:sqref>
+          <xm:sqref>B71:B122 B5:B68</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3946,7 +4145,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formatierung und Schreibweise des Testplans verbessert, manches rausgenommen. Aktualisierung des Inhalts folgt
</commit_message>
<xml_diff>
--- a/Testplan.xlsx
+++ b/Testplan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="335">
   <si>
     <t>Testplan</t>
   </si>
@@ -244,9 +249,6 @@
     <t>Stadt rotiert schneller</t>
   </si>
   <si>
-    <t>MouseOver</t>
-  </si>
-  <si>
     <t>Rechte Maustaste gedrückt halten und die Stadt ziehen</t>
   </si>
   <si>
@@ -400,12 +402,6 @@
     <t>es gibt Daten mit Höhe, Breite = 0</t>
   </si>
   <si>
-    <t>Mit der Maus auf ein Gebäude bzw. Distrikt halten</t>
-  </si>
-  <si>
-    <t>Das Gebäude bzw. Distrikt färbt sich pink</t>
-  </si>
-  <si>
     <t>Vorschau anzeigen</t>
   </si>
   <si>
@@ -470,9 +466,6 @@
   </si>
   <si>
     <t>die Stadt wird angezeigt und in der Bearbeitung wurde etwas geändert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gebäudeinformationen werden eingeblendet und die Option ein Gebäude zu löschen </t>
   </si>
   <si>
     <t>Gebäude wurde angeklickt und die "Gebäudeinformationen" ist geöffnet</t>
@@ -868,9 +861,6 @@
     <t>Zahl-Buchstabe-Zahl-Einträge</t>
   </si>
   <si>
-    <t>Einträge indem zwischen Zahlen Buchstaben stehen</t>
-  </si>
-  <si>
     <t>Es wird die Zahl bis zum ersten auftauchenden Buchstaben gelesen und mit diesem Wert wird das Gebäude gezeichnet</t>
   </si>
   <si>
@@ -970,15 +960,9 @@
     <t>Auf "Experimentelle Version anschalten" klicken</t>
   </si>
   <si>
-    <t>Es werden weitere Funktionalitäten für die Stadtansicht freigeschaltet, Achtung: Funktionalitäten sind nicht bugfrei. Es kann zu fehlerhaften Darstellungen kommen</t>
-  </si>
-  <si>
     <t>Blöcke auswählen</t>
   </si>
   <si>
-    <t>PunktBlockbildung</t>
-  </si>
-  <si>
     <t>Klicken auf "Es wird nach jedem Punkt eine neue Ebene gebildet"</t>
   </si>
   <si>
@@ -1055,6 +1039,18 @@
   </si>
   <si>
     <t>Das fixierte Gebäude, welches durch die Gebäudesuche gefunden wurde, wird wieder deaktiviert</t>
+  </si>
+  <si>
+    <t>Einträge, bei denen zwischen Zahlen Buchstaben stehen</t>
+  </si>
+  <si>
+    <t>Es werden weitere Funktionalitäten für die Stadtansicht freigeschaltet, Achtung: Funktionalitäten sind nicht fehlerfrei. Es kann zu fehlerhaften Darstellungen kommen</t>
+  </si>
+  <si>
+    <t>Punkt-Blockbildung</t>
+  </si>
+  <si>
+    <t>Gebäudeinformationen werden eingeblendet</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1269,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1358,9 +1354,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1388,6 +1381,39 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1409,38 +1435,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1716,7 +1727,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1726,37 +1737,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C124" sqref="C124"/>
+      <selection pane="bottomRight" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="80.33203125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="6.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="10"/>
+    <col min="1" max="1" width="20.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="80.28515625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="9"/>
@@ -1765,17 +1776,17 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="55"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="8"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
@@ -1812,1358 +1823,1358 @@
       <c r="U3" s="28"/>
       <c r="V3" s="28"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-    </row>
-    <row r="5" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+    </row>
+    <row r="5" spans="1:22" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-    </row>
-    <row r="6" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="56"/>
+      <c r="G6" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="33" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    </row>
+    <row r="7" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="G7" s="17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="33" t="s">
-        <v>107</v>
+      <c r="E10" s="32" t="s">
+        <v>106</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>92</v>
+        <v>148</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="33" t="s">
-        <v>107</v>
+      <c r="E11" s="32" t="s">
+        <v>106</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>38</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+    </row>
+    <row r="13" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:22" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="G13" s="17" t="s">
+    </row>
+    <row r="15" spans="1:22" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="62"/>
+    </row>
+    <row r="23" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="F23" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="17" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>225</v>
-      </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="33" t="s">
+      <c r="G24" s="17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
+      <c r="B25" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="D25" s="25"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="34" t="s">
+      <c r="G25" s="17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="25"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27" s="25"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>264</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="34" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="17" t="s">
+      <c r="G28" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="G26" s="17" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="33" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" s="34" t="s">
+      <c r="D29" s="25"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="17" t="s">
+      <c r="G29" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="G27" s="17" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="34" t="s">
+      <c r="D30" s="25"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="17" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="D31" s="25"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="17" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C29" s="34" t="s">
+      <c r="G31" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="17" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="17" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="34" t="s">
+      <c r="G32" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>280</v>
-      </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+    </row>
+    <row r="33" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-    </row>
-    <row r="33" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="B33" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+    </row>
+    <row r="34" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" s="33" t="s">
+      <c r="B34" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="33" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F34" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="33" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33" t="s">
+      <c r="G34" s="32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="33" t="s">
+      <c r="B35" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33" t="s">
+      <c r="D35" s="32"/>
+      <c r="E35" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="G35" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="G36" s="36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="25"/>
+      <c r="E37" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
+    </row>
+    <row r="38" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>294</v>
-      </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37" t="s">
-        <v>295</v>
-      </c>
-      <c r="F35" s="37" t="s">
-        <v>296</v>
-      </c>
-      <c r="G35" s="37" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="33" t="s">
+      <c r="B38" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="E38" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="33" t="s">
+      <c r="B39" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="25"/>
+      <c r="E39" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="25"/>
+      <c r="E40" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="25"/>
+      <c r="E41" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="38"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+    </row>
+    <row r="44" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="32"/>
+      <c r="E44" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="G36" s="33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="33" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="F39" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39" t="s">
-        <v>308</v>
-      </c>
-      <c r="G41" s="39" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
+      <c r="F44" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-    </row>
-    <row r="43" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="33"/>
-      <c r="E43" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="33" t="s">
+      <c r="G44" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="G43" s="33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="G44" s="33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
-        <v>112</v>
+    </row>
+    <row r="45" spans="1:7" s="11" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>132</v>
+        <v>148</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>129</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="G45" s="33" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>134</v>
+        <v>148</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>129</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="F46" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="G46" s="33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="32" t="s">
-        <v>112</v>
+        <v>176</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="11" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>199</v>
+        <v>148</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>131</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="F47" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="G47" s="33" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="11" customFormat="1" ht="57" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="32" t="s">
-        <v>334</v>
+        <v>194</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>220</v>
+        <v>148</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>195</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="F48" s="33" t="s">
-        <v>322</v>
-      </c>
-      <c r="G48" s="33" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="38" t="s">
-        <v>112</v>
+        <v>196</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="11" customFormat="1" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="31" t="s">
+        <v>327</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="39" t="s">
-        <v>323</v>
+        <v>148</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="F49" s="39" t="s">
-        <v>325</v>
-      </c>
-      <c r="G49" s="39" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="11" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="36" t="s">
-        <v>112</v>
+        <v>198</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" s="37" t="s">
-        <v>298</v>
+        <v>148</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>316</v>
       </c>
       <c r="D50" s="25"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="37" t="s">
-        <v>299</v>
-      </c>
-      <c r="G50" s="37" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
-        <v>112</v>
+      <c r="E50" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="F50" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="G50" s="38" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="11" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>111</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>205</v>
+        <v>148</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>293</v>
       </c>
       <c r="D51" s="25"/>
-      <c r="E51" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="F51" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="G51" s="33" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="32" t="s">
-        <v>112</v>
+      <c r="E51" s="17"/>
+      <c r="F51" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>203</v>
+        <v>148</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>201</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="F52" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="G52" s="33" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
-        <v>112</v>
+        <v>194</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" s="33" t="s">
-        <v>203</v>
+        <v>148</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>199</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="F53" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="32" t="s">
-        <v>112</v>
+        <v>203</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="33" t="s">
-        <v>203</v>
+        <v>148</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>199</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="F54" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="G54" s="33" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="32" t="s">
-        <v>112</v>
+        <v>208</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B55" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="D55" s="25"/>
+      <c r="E55" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="32"/>
+      <c r="E56" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="11" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="D57" s="38"/>
+      <c r="E57" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="F57" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="G57" s="38" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="D58" s="32"/>
+      <c r="E58" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D59" s="32"/>
+      <c r="E59" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="G59" s="32" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="C55" s="33" t="s">
+      <c r="D60" s="32"/>
+      <c r="E60" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C61" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="33"/>
-      <c r="E55" s="17" t="s">
+      <c r="D61" s="32"/>
+      <c r="E61" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F55" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="G55" s="33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C56" s="39" t="s">
+      <c r="F61" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" s="32"/>
+      <c r="E62" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="11" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="D63" s="40"/>
+      <c r="E63" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="F63" s="41" t="s">
         <v>311</v>
       </c>
-      <c r="D56" s="39"/>
-      <c r="E56" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="F56" s="39" t="s">
+      <c r="G63" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="G56" s="39" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" s="11" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="D57" s="33"/>
-      <c r="E57" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="F57" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="G57" s="33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C58" s="33" t="s">
+    </row>
+    <row r="64" spans="1:7" s="11" customFormat="1" ht="39" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="33"/>
-      <c r="E58" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="F58" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="G58" s="33" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="D59" s="33"/>
-      <c r="E59" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F59" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="G59" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C60" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G60" s="33" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="D61" s="33"/>
-      <c r="E61" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="F61" s="33" t="s">
+      <c r="F64" s="54"/>
+      <c r="G64" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="G61" s="33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>317</v>
-      </c>
-      <c r="D62" s="56"/>
-      <c r="E62" s="57" t="s">
-        <v>320</v>
-      </c>
-      <c r="F62" s="57" t="s">
-        <v>318</v>
-      </c>
-      <c r="G62" s="39" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" s="11" customFormat="1" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C63" s="33" t="s">
+      <c r="D65" s="32"/>
+      <c r="E65" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="11" customFormat="1" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" s="32"/>
+      <c r="E66" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F66" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="43" t="s">
+    </row>
+    <row r="67" spans="1:7" s="11" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+    </row>
+    <row r="68" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G68" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="F63" s="44"/>
-      <c r="G63" s="33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" s="33"/>
-      <c r="E64" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F64" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G64" s="33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="11" customFormat="1" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D65" s="33"/>
-      <c r="E65" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F65" s="33" t="s">
+      <c r="F69" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G69" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="14.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="45"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="47"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="G65" s="33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-    </row>
-    <row r="67" spans="1:7" ht="22.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C67" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" s="33"/>
-      <c r="E67" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="F67" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G67" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="34.200000000000003" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D68" s="33"/>
-      <c r="E68" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="F68" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G68" s="33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="14.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="50"/>
-      <c r="B69" s="51"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="51"/>
-      <c r="E69" s="51"/>
-      <c r="F69" s="51"/>
-      <c r="G69" s="52"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="B70" s="48"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="49"/>
-    </row>
-    <row r="71" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="21" t="s">
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="44"/>
+    </row>
+    <row r="72" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B71" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="40"/>
-      <c r="F71" s="40"/>
-      <c r="G71" s="40"/>
-    </row>
-    <row r="72" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C72" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="22"/>
-      <c r="E72" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F72" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G72" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" s="50"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="50"/>
+    </row>
+    <row r="73" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C73" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D73" s="22"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="E73" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F73" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G73" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C74" s="23" t="s">
         <v>14</v>
@@ -3172,15 +3183,15 @@
       <c r="E74" s="23"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C75" s="23" t="s">
         <v>14</v>
@@ -3192,12 +3203,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C76" s="23" t="s">
         <v>14</v>
@@ -3206,142 +3217,140 @@
       <c r="E76" s="23"/>
       <c r="F76" s="15"/>
       <c r="G76" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C77" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="22"/>
-      <c r="E77" s="23" t="s">
-        <v>160</v>
-      </c>
+      <c r="E77" s="23"/>
       <c r="F77" s="15"/>
       <c r="G77" s="15" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C78" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="22"/>
-      <c r="E78" s="23"/>
+      <c r="E78" s="23" t="s">
+        <v>156</v>
+      </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D79" s="17"/>
-      <c r="E79" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="C79" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="D80" s="17"/>
       <c r="E80" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F80" s="23"/>
       <c r="G80" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="17"/>
+      <c r="E81" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B81" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="23" t="s">
+      <c r="B82" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="23"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F81" s="54"/>
-      <c r="G81" s="54"/>
-    </row>
-    <row r="82" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C82" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F82" s="49"/>
+      <c r="G82" s="49"/>
+    </row>
+    <row r="83" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G83" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F83" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C84" s="23" t="s">
         <v>20</v>
@@ -3349,111 +3358,111 @@
       <c r="D84" s="22"/>
       <c r="E84" s="23"/>
       <c r="F84" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G84" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="23"/>
       <c r="F85" s="23" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="G85" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="23"/>
       <c r="F86" s="23" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="G86" s="23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C87" s="39" t="s">
-        <v>328</v>
-      </c>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="39" t="s">
-        <v>329</v>
-      </c>
-      <c r="G87" s="39" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="C87" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="G87" s="38" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B88" s="30" t="s">
-        <v>152</v>
+      <c r="B88" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D88" s="25"/>
       <c r="E88" s="23" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F88" s="23" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G88" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="26.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C89" s="23"/>
       <c r="D89" s="22"/>
       <c r="E89" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F89" s="54"/>
-      <c r="G89" s="54"/>
-    </row>
-    <row r="90" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="F89" s="49"/>
+      <c r="G89" s="49"/>
+    </row>
+    <row r="90" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C90" s="23" t="s">
         <v>26</v>
@@ -3461,18 +3470,18 @@
       <c r="D90" s="22"/>
       <c r="E90" s="23"/>
       <c r="F90" s="23" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="G90" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="91" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C91" s="23" t="s">
         <v>27</v>
@@ -3486,12 +3495,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C92" s="23" t="s">
         <v>27</v>
@@ -3500,36 +3509,36 @@
       <c r="E92" s="23"/>
       <c r="F92" s="23"/>
       <c r="G92" s="23" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C93" s="29" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F93" s="29" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G93" s="29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C94" s="23" t="s">
         <v>29</v>
@@ -3540,15 +3549,15 @@
         <v>48</v>
       </c>
       <c r="G94" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C95" s="23" t="s">
         <v>29</v>
@@ -3559,15 +3568,15 @@
       </c>
       <c r="F95" s="23"/>
       <c r="G95" s="23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C96" s="23" t="s">
         <v>29</v>
@@ -3583,12 +3592,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C97" s="23" t="s">
         <v>29</v>
@@ -3604,75 +3613,75 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="57" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D98" s="25"/>
       <c r="E98" s="23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F98" s="23" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G98" s="23" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="23" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F99" s="23" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G99" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D100" s="25"/>
       <c r="E100" s="25" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F100" s="23" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="G100" s="23" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="22" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C101" s="23" t="s">
         <v>56</v>
@@ -3686,33 +3695,33 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="22" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C102" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D102" s="22"/>
       <c r="E102" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F102" s="23" t="s">
         <v>59</v>
       </c>
       <c r="G102" s="23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C103" s="23" t="s">
         <v>56</v>
@@ -3721,36 +3730,36 @@
       <c r="E103" s="23"/>
       <c r="F103" s="23"/>
       <c r="G103" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="22" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C104" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F104" s="23" t="s">
         <v>60</v>
       </c>
       <c r="G104" s="23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C105" s="23" t="s">
         <v>56</v>
@@ -3759,22 +3768,22 @@
       <c r="E105" s="23"/>
       <c r="F105" s="23"/>
       <c r="G105" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="24" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C106" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D106" s="22"/>
       <c r="E106" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F106" s="23" t="s">
         <v>61</v>
@@ -3783,12 +3792,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="107" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C107" s="23" t="s">
         <v>63</v>
@@ -3802,12 +3811,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C108" s="23" t="s">
         <v>63</v>
@@ -3821,12 +3830,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C109" s="23" t="s">
         <v>63</v>
@@ -3840,12 +3849,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C110" s="23" t="s">
         <v>63</v>
@@ -3859,12 +3868,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C111" s="23" t="s">
         <v>63</v>
@@ -3878,150 +3887,150 @@
         <v>73</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="37" t="s">
+    <row r="112" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="36" t="s">
         <v>26</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C112" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C112" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="D112" s="37"/>
-      <c r="E112" s="37"/>
-      <c r="F112" s="37" t="s">
-        <v>292</v>
-      </c>
-      <c r="G112" s="37" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D112" s="36"/>
+      <c r="E112" s="36"/>
+      <c r="F112" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="G112" s="36" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D113" s="22"/>
       <c r="E113" s="23"/>
       <c r="F113" s="23" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G113" s="23" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="22.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="38" t="s">
         <v>26</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C114" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="D114" s="39"/>
-      <c r="E114" s="39" t="s">
-        <v>335</v>
-      </c>
-      <c r="F114" s="39" t="s">
-        <v>336</v>
-      </c>
-      <c r="G114" s="39" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="C114" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="D114" s="38"/>
+      <c r="E114" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="F114" s="38" t="s">
+        <v>329</v>
+      </c>
+      <c r="G114" s="38" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D115" s="22"/>
       <c r="E115" s="23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F115" s="23" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G115" s="23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D116" s="22"/>
       <c r="E116" s="23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F116" s="23" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G116" s="23" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="48" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D117" s="22"/>
       <c r="E117" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F117" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="F117" s="23" t="s">
-        <v>169</v>
-      </c>
       <c r="G117" s="23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C118" s="48"/>
+      <c r="D118" s="48"/>
+      <c r="E118" s="48"/>
+      <c r="F118" s="48"/>
+      <c r="G118" s="48"/>
+    </row>
+    <row r="119" spans="1:7" s="20" customFormat="1" ht="36" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C119" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="B118" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C118" s="53"/>
-      <c r="D118" s="53"/>
-      <c r="E118" s="53"/>
-      <c r="F118" s="53"/>
-      <c r="G118" s="53"/>
-    </row>
-    <row r="119" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B119" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C119" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="23"/>
@@ -4029,84 +4038,86 @@
         <v>30</v>
       </c>
       <c r="G119" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="20" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C120" s="23" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" s="20" customFormat="1" ht="45.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B120" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C120" s="23" t="s">
-        <v>85</v>
       </c>
       <c r="D120" s="22"/>
       <c r="E120" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F120" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="F120" s="23" t="s">
+      <c r="G120" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G120" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="20" customFormat="1" ht="34.200000000000003" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="37" t="s">
-        <v>82</v>
+    </row>
+    <row r="121" spans="1:7" s="20" customFormat="1" ht="36" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C121" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="D121" s="37"/>
-      <c r="E121" s="37" t="s">
-        <v>327</v>
-      </c>
-      <c r="F121" s="37" t="s">
-        <v>304</v>
-      </c>
-      <c r="G121" s="37" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A122" s="38" t="s">
-        <v>82</v>
+        <v>148</v>
+      </c>
+      <c r="C121" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D121" s="36"/>
+      <c r="E121" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="F121" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="G121" s="36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C122" s="37" t="s">
-        <v>301</v>
-      </c>
-      <c r="F122" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="G122" s="37" t="s">
-        <v>303</v>
+        <v>148</v>
+      </c>
+      <c r="C122" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="F122" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="G122" s="36" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="C71:G71"/>
+  <mergeCells count="16">
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="C67:G67"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="E64:F64"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="C72:G72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4117,7 +4128,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B71:B122 B5:B68</xm:sqref>
+          <xm:sqref>B5:B69 B72:B122</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4133,9 +4144,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -4145,7 +4156,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>